<commit_message>
Add ingame base systems.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Documents/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E8EDBF-D59B-A142-BE1C-4160F638CBE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07BEF54-3079-F848-8CA7-B49BBF6EF1E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage" sheetId="1" r:id="rId1"/>
+    <sheet name="Character" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
@@ -46,6 +47,24 @@
   </si>
   <si>
     <t>field_test</t>
+  </si>
+  <si>
+    <t>assetName</t>
+  </si>
+  <si>
+    <t>chr_test</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>radius</t>
+  </si>
+  <si>
+    <t>moveSpeed</t>
   </si>
 </sst>
 </file>
@@ -422,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28CFC96-440A-0B49-975F-088F9B4F16E5}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,10 +477,95 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>101</v>
+        <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD673615-854F-D74F-BA9C-3B86DF648DEE}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="5" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add functions to create characte objects.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Documents/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07BEF54-3079-F848-8CA7-B49BBF6EF1E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795A86E1-3472-AD46-98F4-8E8AF7407945}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -55,16 +55,13 @@
     <t>chr_test</t>
   </si>
   <si>
-    <t>height</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
-    <t>radius</t>
-  </si>
-  <si>
     <t>moveSpeed</t>
+  </si>
+  <si>
+    <t>weight</t>
   </si>
 </sst>
 </file>
@@ -490,20 +487,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD673615-854F-D74F-BA9C-3B86DF648DEE}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="5" width="14.5" customWidth="1"/>
+    <col min="3" max="4" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -511,30 +508,25 @@
         <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -542,16 +534,13 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -559,13 +548,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E5" s="2">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a character action 'Move'.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Documents/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795A86E1-3472-AD46-98F4-8E8AF7407945}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FB0E94-1885-234E-BA09-C53F381F39BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>id</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>weight</t>
+  </si>
+  <si>
+    <t>jumpPower</t>
   </si>
 </sst>
 </file>
@@ -487,20 +490,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD673615-854F-D74F-BA9C-3B86DF648DEE}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="4" width="14.5" customWidth="1"/>
+    <col min="3" max="5" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,20 +516,25 @@
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -539,8 +547,11 @@
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -548,10 +559,13 @@
         <v>6</v>
       </c>
       <c r="C5" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D5" s="2">
         <v>50</v>
+      </c>
+      <c r="E5" s="2">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add a character action 'Jump'.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Documents/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FB0E94-1885-234E-BA09-C53F381F39BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F00C98B-164A-2943-97A0-AAD4A4EE672C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -64,7 +64,29 @@
     <t>weight</t>
   </si>
   <si>
-    <t>jumpPower</t>
+    <t>int</t>
+  </si>
+  <si>
+    <t>jumpMaxCount</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>None = 0,
+Normal = 1,</t>
+  </si>
+  <si>
+    <t>fieldGravity</t>
+  </si>
+  <si>
+    <t>FieldGravity</t>
+  </si>
+  <si>
+    <t>jumpHeight</t>
   </si>
 </sst>
 </file>
@@ -121,10 +143,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,48 +464,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28CFC96-440A-0B49-975F-088F9B4F16E5}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -490,20 +529,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD673615-854F-D74F-BA9C-3B86DF648DEE}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="5" width="14.5" customWidth="1"/>
+    <col min="3" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,27 +553,42 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -550,8 +604,17 @@
       <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -562,10 +625,19 @@
         <v>20</v>
       </c>
       <c r="D5" s="2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E5" s="2">
+        <v>150</v>
+      </c>
+      <c r="F5" s="2">
         <v>100</v>
+      </c>
+      <c r="G5" s="2">
+        <v>200</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added base gimmick systems.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Documents/chsopoly-client/Excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Projects/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0C2528-FEB0-B343-A480-E9C2E2243C4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9458633-1C21-4348-BA10-DAC64601D411}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage" sheetId="1" r:id="rId1"/>
     <sheet name="Character" sheetId="2" r:id="rId2"/>
+    <sheet name="Gimmick" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -65,12 +66,6 @@
   </si>
   <si>
     <t>int</t>
-  </si>
-  <si>
-    <t>width</t>
-  </si>
-  <si>
-    <t>height</t>
   </si>
   <si>
     <t>None = 0,
@@ -87,6 +82,18 @@
   </si>
   <si>
     <t>aerialJumpCount</t>
+  </si>
+  <si>
+    <t>lotteryWeight</t>
+  </si>
+  <si>
+    <t>gim_test1</t>
+  </si>
+  <si>
+    <t>gim_test2</t>
+  </si>
+  <si>
+    <t>gim_test3</t>
   </si>
 </sst>
 </file>
@@ -467,7 +474,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,7 +492,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -497,7 +504,7 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -508,7 +515,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -529,20 +536,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD673615-854F-D74F-BA9C-3B86DF648DEE}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="8" width="14.5" customWidth="1"/>
+    <col min="3" max="6" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,42 +560,32 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -605,16 +602,10 @@
         <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -628,15 +619,94 @@
         <v>100</v>
       </c>
       <c r="E5" s="2">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="F5" s="2">
-        <v>100</v>
-      </c>
-      <c r="G5" s="2">
-        <v>200</v>
-      </c>
-      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F26C27-2840-7340-B9E1-2A96B12E88DA}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed: Unable to load 'gim_wood_step'.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Projects/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1541776-5395-AC46-898A-16F23A25B839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A3E63E-1766-F34B-B4A9-139E266FCE1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,7 +629,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add a character/gimmick action to destroy a target gimmick.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Projects/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A3E63E-1766-F34B-B4A9-139E266FCE1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD60047C-31BD-0C4F-AF5B-DAA3926442D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19260" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>id</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>gim_wood_step</t>
+  </si>
+  <si>
+    <t>hitPoint</t>
+  </si>
+  <si>
+    <t>power</t>
   </si>
 </sst>
 </file>
@@ -530,20 +536,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD673615-854F-D74F-BA9C-3B86DF648DEE}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="J18" sqref="J17:J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="6" width="14.5" customWidth="1"/>
+    <col min="3" max="7" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -562,24 +568,29 @@
       <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -598,8 +609,11 @@
       <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -617,6 +631,9 @@
       </c>
       <c r="F5" s="2">
         <v>1</v>
+      </c>
+      <c r="G5" s="2">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -626,20 +643,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F26C27-2840-7340-B9E1-2A96B12E88DA}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="3" max="4" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,18 +666,23 @@
       <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -670,8 +692,11 @@
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -680,6 +705,9 @@
       </c>
       <c r="C5" s="2">
         <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Wait for gimmick box gauge to put a gimmick.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Projects/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD60047C-31BD-0C4F-AF5B-DAA3926442D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D2E735-0838-4E49-AE0C-C414404B3F65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19260" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19260" activeTab="2" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>id</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>power</t>
+  </si>
+  <si>
+    <t>coolTime</t>
   </si>
 </sst>
 </file>
@@ -538,8 +541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD673615-854F-D74F-BA9C-3B86DF648DEE}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J17:J18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -643,20 +646,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F26C27-2840-7340-B9E1-2A96B12E88DA}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="4" width="13.83203125" customWidth="1"/>
+    <col min="3" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,20 +672,25 @@
       <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -695,8 +703,11 @@
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -707,6 +718,9 @@
         <v>1</v>
       </c>
       <c r="D5" s="2">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Able to attack to characters from gimmick objects.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Projects/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D2E735-0838-4E49-AE0C-C414404B3F65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B43ACD1-4849-724B-97DD-87AEA78405CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19260" activeTab="2" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" activeTab="2" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>id</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>coolTime</t>
+  </si>
+  <si>
+    <t>damage</t>
+  </si>
+  <si>
+    <t>gim_damage_wood_step</t>
+  </si>
+  <si>
+    <t>hp</t>
   </si>
 </sst>
 </file>
@@ -539,20 +548,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD673615-854F-D74F-BA9C-3B86DF648DEE}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E30" sqref="E30:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="7" width="14.5" customWidth="1"/>
+    <col min="3" max="8" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,8 +583,11 @@
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -583,8 +595,9 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -592,8 +605,9 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -615,8 +629,11 @@
       <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -637,6 +654,9 @@
       </c>
       <c r="G5" s="2">
         <v>2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -646,20 +666,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F26C27-2840-7340-B9E1-2A96B12E88DA}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="5" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="6" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,22 +695,27 @@
       <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -706,8 +731,11 @@
       <c r="E4" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -722,6 +750,29 @@
       </c>
       <c r="E5" s="2">
         <v>5</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add timer on ingame.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Projects/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B43ACD1-4849-724B-97DD-87AEA78405CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68A98E9-46E7-4B4B-8943-C7A910149D90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" activeTab="2" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>id</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>hp</t>
+  </si>
+  <si>
+    <t>limitTime</t>
   </si>
 </sst>
 </file>
@@ -483,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28CFC96-440A-0B49-975F-088F9B4F16E5}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -494,9 +497,10 @@
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="4" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,20 +510,25 @@
       <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -529,8 +538,11 @@
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -540,9 +552,13 @@
       <c r="C5" s="2">
         <v>1</v>
       </c>
+      <c r="D5" s="2">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -551,7 +567,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30:E31"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F26C27-2840-7340-B9E1-2A96B12E88DA}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Renamed gim_damage_wood_step to gim_rolling_saw.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Projects/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68A98E9-46E7-4B4B-8943-C7A910149D90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339E168F-E38A-7641-8E0F-7419878F8D1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" activeTab="2" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage" sheetId="1" r:id="rId1"/>
@@ -102,13 +102,13 @@
     <t>damage</t>
   </si>
   <si>
-    <t>gim_damage_wood_step</t>
-  </si>
-  <si>
     <t>hp</t>
   </si>
   <si>
     <t>limitTime</t>
+  </si>
+  <si>
+    <t>gim_rolling_saw</t>
   </si>
 </sst>
 </file>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28CFC96-440A-0B49-975F-088F9B4F16E5}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -511,7 +511,7 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -600,7 +600,7 @@
         <v>19</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F26C27-2840-7340-B9E1-2A96B12E88DA}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -776,7 +776,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>

</xml_diff>

<commit_message>
Popup system was added.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Projects/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339E168F-E38A-7641-8E0F-7419878F8D1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C14A939-E8AD-714A-8F5D-79D4965CFF5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" activeTab="2" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>gim_rolling_saw</t>
+  </si>
+  <si>
+    <t>chr_bird</t>
   </si>
 </sst>
 </file>
@@ -564,10 +567,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD673615-854F-D74F-BA9C-3B86DF648DEE}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -675,6 +678,32 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2">
+        <v>400</v>
+      </c>
+      <c r="D6" s="2">
+        <v>100</v>
+      </c>
+      <c r="E6" s="2">
+        <v>200</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2">
+        <v>2</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -684,7 +713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F26C27-2840-7340-B9E1-2A96B12E88DA}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add frog to master data.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Projects/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C14A939-E8AD-714A-8F5D-79D4965CFF5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231E05DD-040E-9046-8675-7106DAC26281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>chr_bird</t>
+  </si>
+  <si>
+    <t>chr_frog</t>
   </si>
 </sst>
 </file>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD673615-854F-D74F-BA9C-3B86DF648DEE}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,6 +704,32 @@
         <v>2</v>
       </c>
       <c r="H6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2">
+        <v>400</v>
+      </c>
+      <c r="D7" s="2">
+        <v>100</v>
+      </c>
+      <c r="E7" s="2">
+        <v>200</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>2</v>
+      </c>
+      <c r="H7" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Ingame character data.
</commit_message>
<xml_diff>
--- a/Excels/Ingame.xlsx
+++ b/Excels/Ingame.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/s-tanikawa/Projects/chsopoly-client/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231E05DD-040E-9046-8675-7106DAC26281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CF60DE-9C35-AC46-ACE2-389B863500FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19120" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
+    <workbookView xWindow="42980" yWindow="2000" windowWidth="33600" windowHeight="19120" activeTab="1" xr2:uid="{80F27EA5-0B5F-334F-ACE1-0B827E15297F}"/>
   </bookViews>
   <sheets>
     <sheet name="Stage" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>id</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>chr_frog</t>
+  </si>
+  <si>
+    <t>chr_deer</t>
+  </si>
+  <si>
+    <t>chr_mouse</t>
   </si>
 </sst>
 </file>
@@ -570,10 +576,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD673615-854F-D74F-BA9C-3B86DF648DEE}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,6 +736,58 @@
         <v>2</v>
       </c>
       <c r="H7" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="2">
+        <v>400</v>
+      </c>
+      <c r="D8" s="2">
+        <v>100</v>
+      </c>
+      <c r="E8" s="2">
+        <v>200</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>2</v>
+      </c>
+      <c r="H8" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="2">
+        <v>400</v>
+      </c>
+      <c r="D9" s="2">
+        <v>100</v>
+      </c>
+      <c r="E9" s="2">
+        <v>200</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1</v>
+      </c>
+      <c r="G9" s="2">
+        <v>2</v>
+      </c>
+      <c r="H9" s="2">
         <v>3</v>
       </c>
     </row>

</xml_diff>